<commit_message>
added new results from spider 1 with scrape date
</commit_message>
<xml_diff>
--- a/ZorgkaartScrapy/data/zorgkaart_organisatietypes.xlsx
+++ b/ZorgkaartScrapy/data/zorgkaart_organisatietypes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>aantal</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>scraped_at</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -464,6 +469,11 @@
       <c r="C2" t="n">
         <v>5031</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -479,6 +489,11 @@
       <c r="C3" t="n">
         <v>18</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -494,6 +509,11 @@
       <c r="C4" t="n">
         <v>1945</v>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -509,6 +529,11 @@
       <c r="C5" t="n">
         <v>531</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -524,6 +549,11 @@
       <c r="C6" t="n">
         <v>392</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -539,6 +569,11 @@
       <c r="C7" t="n">
         <v>5</v>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -554,6 +589,11 @@
       <c r="C8" t="n">
         <v>45</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -569,6 +609,11 @@
       <c r="C9" t="n">
         <v>39</v>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -584,6 +629,11 @@
       <c r="C10" t="n">
         <v>42</v>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -599,6 +649,11 @@
       <c r="C11" t="n">
         <v>5</v>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -614,6 +669,11 @@
       <c r="C12" t="n">
         <v>12</v>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -629,6 +689,11 @@
       <c r="C13" t="n">
         <v>3</v>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -644,6 +709,11 @@
       <c r="C14" t="n">
         <v>56</v>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -659,6 +729,11 @@
       <c r="C15" t="n">
         <v>29</v>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -674,6 +749,11 @@
       <c r="C16" t="n">
         <v>852</v>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -689,6 +769,11 @@
       <c r="C17" t="n">
         <v>67</v>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -704,6 +789,11 @@
       <c r="C18" t="n">
         <v>92</v>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -719,6 +809,11 @@
       <c r="C19" t="n">
         <v>3665</v>
       </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -734,6 +829,11 @@
       <c r="C20" t="n">
         <v>103</v>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -749,6 +849,11 @@
       <c r="C21" t="n">
         <v>26</v>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -764,6 +869,11 @@
       <c r="C22" t="n">
         <v>816</v>
       </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -779,6 +889,11 @@
       <c r="C23" t="n">
         <v>70</v>
       </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -794,6 +909,11 @@
       <c r="C24" t="n">
         <v>9957</v>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -809,6 +929,11 @@
       <c r="C25" t="n">
         <v>65</v>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -824,6 +949,11 @@
       <c r="C26" t="n">
         <v>2100</v>
       </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -839,6 +969,11 @@
       <c r="C27" t="n">
         <v>155</v>
       </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -854,6 +989,11 @@
       <c r="C28" t="n">
         <v>192</v>
       </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -869,6 +1009,11 @@
       <c r="C29" t="n">
         <v>726</v>
       </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -884,6 +1029,11 @@
       <c r="C30" t="n">
         <v>108</v>
       </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -899,6 +1049,11 @@
       <c r="C31" t="n">
         <v>4831</v>
       </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -914,6 +1069,11 @@
       <c r="C32" t="n">
         <v>9</v>
       </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -929,6 +1089,11 @@
       <c r="C33" t="n">
         <v>164</v>
       </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -944,6 +1109,11 @@
       <c r="C34" t="n">
         <v>356</v>
       </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -959,6 +1129,11 @@
       <c r="C35" t="n">
         <v>3</v>
       </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -974,6 +1149,11 @@
       <c r="C36" t="n">
         <v>1192</v>
       </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -989,6 +1169,11 @@
       <c r="C37" t="n">
         <v>3070</v>
       </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1004,6 +1189,11 @@
       <c r="C38" t="n">
         <v>991</v>
       </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1019,6 +1209,11 @@
       <c r="C39" t="n">
         <v>62</v>
       </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1034,6 +1229,11 @@
       <c r="C40" t="n">
         <v>727</v>
       </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1049,6 +1249,11 @@
       <c r="C41" t="n">
         <v>1350</v>
       </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1064,6 +1269,11 @@
       <c r="C42" t="n">
         <v>112</v>
       </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1079,6 +1289,11 @@
       <c r="C43" t="n">
         <v>342</v>
       </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1094,6 +1309,11 @@
       <c r="C44" t="n">
         <v>7</v>
       </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1109,6 +1329,11 @@
       <c r="C45" t="n">
         <v>912</v>
       </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1124,6 +1349,11 @@
       <c r="C46" t="n">
         <v>629</v>
       </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1139,6 +1369,11 @@
       <c r="C47" t="n">
         <v>295</v>
       </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1154,6 +1389,11 @@
       <c r="C48" t="n">
         <v>340</v>
       </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1169,6 +1409,11 @@
       <c r="C49" t="n">
         <v>2050</v>
       </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1184,6 +1429,11 @@
       <c r="C50" t="n">
         <v>357</v>
       </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1199,6 +1449,11 @@
       <c r="C51" t="n">
         <v>18</v>
       </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1214,6 +1469,11 @@
       <c r="C52" t="n">
         <v>3536</v>
       </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1229,6 +1489,11 @@
       <c r="C53" t="n">
         <v>233</v>
       </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1244,6 +1509,11 @@
       <c r="C54" t="n">
         <v>4634</v>
       </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1259,6 +1529,11 @@
       <c r="C55" t="n">
         <v>344</v>
       </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1274,6 +1549,11 @@
       <c r="C56" t="n">
         <v>44</v>
       </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1289,6 +1569,11 @@
       <c r="C57" t="n">
         <v>1134</v>
       </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1304,6 +1589,11 @@
       <c r="C58" t="n">
         <v>2358</v>
       </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1319,6 +1609,11 @@
       <c r="C59" t="n">
         <v>262</v>
       </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1334,6 +1629,11 @@
       <c r="C60" t="n">
         <v>4523</v>
       </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1349,6 +1649,11 @@
       <c r="C61" t="n">
         <v>2948</v>
       </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1364,6 +1669,11 @@
       <c r="C62" t="n">
         <v>1595</v>
       </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1379,6 +1689,11 @@
       <c r="C63" t="n">
         <v>22</v>
       </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1394,6 +1709,11 @@
       <c r="C64" t="n">
         <v>77</v>
       </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1409,6 +1729,11 @@
       <c r="C65" t="n">
         <v>95</v>
       </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1424,6 +1749,11 @@
       <c r="C66" t="n">
         <v>312</v>
       </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1439,6 +1769,11 @@
       <c r="C67" t="n">
         <v>10</v>
       </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1454,6 +1789,11 @@
       <c r="C68" t="n">
         <v>65</v>
       </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1469,6 +1809,11 @@
       <c r="C69" t="n">
         <v>128</v>
       </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1484,6 +1829,11 @@
       <c r="C70" t="n">
         <v>494</v>
       </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1499,6 +1849,11 @@
       <c r="C71" t="n">
         <v>20</v>
       </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1514,6 +1869,11 @@
       <c r="C72" t="n">
         <v>17</v>
       </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1529,6 +1889,11 @@
       <c r="C73" t="n">
         <v>63</v>
       </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1544,6 +1909,11 @@
       <c r="C74" t="n">
         <v>292</v>
       </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1559,6 +1929,11 @@
       <c r="C75" t="n">
         <v>448</v>
       </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1574,6 +1949,11 @@
       <c r="C76" t="n">
         <v>54</v>
       </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1589,6 +1969,11 @@
       <c r="C77" t="n">
         <v>37</v>
       </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1603,6 +1988,11 @@
       </c>
       <c r="C78" t="n">
         <v>44</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>